<commit_message>
test fixtures food on index
</commit_message>
<xml_diff>
--- a/src/Documentation/Données pour DB/programme%20alim.xlsx
+++ b/src/Documentation/Données pour DB/programme%20alim.xlsx
@@ -550,11 +550,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,7 +886,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -935,7 +935,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="40"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="27">
         <v>150</v>
       </c>
@@ -963,7 +963,7 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="40"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="29">
         <v>100</v>
       </c>
@@ -971,7 +971,7 @@
         <v>43</v>
       </c>
       <c r="E3" s="22">
-        <f t="shared" ref="E2:E17" si="3">IF($C3="","",VLOOKUP($C3,Details,3,FALSE)/VLOOKUP($C3,Details,2,FALSE)*$B3)</f>
+        <f t="shared" ref="E3:E17" si="3">IF($C3="","",VLOOKUP($C3,Details,3,FALSE)/VLOOKUP($C3,Details,2,FALSE)*$B3)</f>
         <v>3.4000000000000004</v>
       </c>
       <c r="F3" s="3">
@@ -993,7 +993,7 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="29">
         <v>100</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
       <c r="E5" s="22" t="str">
@@ -1050,7 +1050,7 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="29"/>
       <c r="C6" s="30"/>
       <c r="E6" s="22" t="s">
@@ -1075,7 +1075,7 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="29"/>
       <c r="C7" s="30"/>
       <c r="E7" s="22" t="str">
@@ -1099,7 +1099,7 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="29"/>
       <c r="C8" s="30"/>
       <c r="E8" s="22" t="str">
@@ -1123,7 +1123,7 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="E9" s="22" t="str">
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="E10" s="22" t="str">
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="E11" s="22" t="str">
@@ -1186,7 +1186,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="E12" s="22" t="str">
@@ -1207,7 +1207,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="E13" s="22" t="str">
@@ -1228,7 +1228,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="29"/>
       <c r="C14" s="30"/>
       <c r="E14" s="22" t="str">
@@ -1251,7 +1251,7 @@
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="29"/>
       <c r="C15" s="30"/>
       <c r="E15" s="22" t="str">
@@ -1275,7 +1275,7 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="29"/>
       <c r="C16" s="30"/>
       <c r="E16" s="22" t="str">
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="13">
@@ -1420,13 +1420,14 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="9" style="5"/>
+    <col min="2" max="2" width="21.26953125" style="5" customWidth="1"/>
+    <col min="3" max="6" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2040,7 +2041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>41</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>